<commit_message>
Add A03 text and P-P plot & Q-Q plot for A02
</commit_message>
<xml_diff>
--- a/Assignments/A02/data.xlsx
+++ b/Assignments/A02/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Polimi\2020-computer-systems-performance-evaluation\Assignments\A02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A76D86-5301-4B12-BDFB-8FE240DC7094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F2E2DA-20C7-4088-94CD-911381784E6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -398,412 +398,412 @@
   <dimension ref="A1:A80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection sqref="A1:A80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1">
-        <v>143.37657753378699</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>83.05180008887001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>515.9312381731628</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>95.555124350942393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>741.30550631579183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>197.50674834591388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
-        <v>127.20853919240679</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>96.195503150980159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
-        <v>452.08657097797015</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>462.55639450800726</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
-        <v>408.24208286158517</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>37.471240162091377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
-        <v>734.48280897932705</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>483.05881266032151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
-        <v>297.05949961458481</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>153.72734732003377</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
-        <v>610.76833651825882</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4.0125320879330129E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
-        <v>171.39313170857503</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>56.484830643113618</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
-        <v>404.09161925463451</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>75.198047766991465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
-        <v>546.05786111395514</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>17.290833278543918</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
-        <v>44.400512762108917</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>150.22282025328411</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
-        <v>567.71401876333539</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>384.74099741048815</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
-        <v>31.086207187404273</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>121.54390135027747</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
-        <v>28.020620459691038</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>95.508472837579603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
-        <v>36.177327000422501</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>55.071393391423193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
-        <v>338.47237654288466</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>204.95000236613504</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
-        <v>7.0687592261761534</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>307.45389067222851</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
-        <v>104.15616379127033</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>39.165941927668449</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
-        <v>93.128334703566225</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>73.217277847827489</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
-        <v>62.704208415380201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>113.77313559557923</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
-        <v>22.926011738335692</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>177.67603202236964</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
-        <v>211.17932007251454</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9.6422963683094594</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
-        <v>204.54072297494861</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>187.40390693335311</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
-        <v>37.381507718147319</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+        <v>55.240466600337804</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
-        <v>17.424032070354862</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+        <v>158.72513290721375</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
-        <v>114.85738548665805</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9.1873165500892089</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
-        <v>87.728895727954978</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+        <v>136.77415928794977</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
-        <v>31.621594689661432</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+        <v>210.12934562121734</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
-        <v>3.3139570394267208</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>143.41200250156683</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
-        <v>0.40339278890970293</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>30.157541258017698</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
-        <v>70.362027587540666</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>331.47910602105378</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
-        <v>34.596030261344488</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>24.240443497544447</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
-        <v>0.75684007027798594</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+        <v>95.057763119825978</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
-        <v>211.26530980185424</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+        <v>100.74696146710146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
-        <v>47.424722750945698</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+        <v>49.342984813101481</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
-        <v>84.697769404210447</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+        <v>86.207529133500515</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
-        <v>36.691705111601749</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+        <v>39.388630657554032</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
-        <v>18.488539827397808</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+        <v>54.622041701904244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
-        <v>9.1508899441639979</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+        <v>71.013179681318164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
-        <v>1.4335186920259384</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+        <v>28.234282091141061</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
-        <v>44.247851856339466</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+        <v>213.12392088489796</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
-        <v>236.66440181322704</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+        <v>41.685653700389068</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
-        <v>179.24943444566139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+        <v>100.13405448969992</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
-        <v>310.37938201551304</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+        <v>551.00863737440886</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
-        <v>103.96347826429135</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+        <v>682.45622475338962</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
-        <v>17.396014719743746</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+        <v>83.054177805473913</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
-        <v>24.129297924539571</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+        <v>82.471470871917063</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
-        <v>22.074793687108645</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+        <v>211.19440817982809</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
-        <v>7.1953776090914383</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+        <v>27.135514363649847</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
-        <v>139.49333344441379</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+        <v>76.056817691185358</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
-        <v>57.22902047466625</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+        <v>205.24619387009525</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
-        <v>8.6077952849726103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+        <v>42.480138444621453</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
-        <v>106.16092939314142</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9.1158842395740916</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
-        <v>13.045413010544852</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+        <v>45.726735112944795</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
-        <v>38.147380410255415</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+        <v>428.04195178722659</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
-        <v>179.47290981637664</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1012.1254766244434</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
-        <v>41.531977008647644</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+        <v>108.43970817258626</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
-        <v>2.6745534416789591</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+        <v>172.13491459069434</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
-        <v>268.00172158144863</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+        <v>296.08203511826349</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
-        <v>41.200008936534616</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+        <v>130.95214582527012</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
-        <v>59.389726446832078</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+        <v>144.09227898729822</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
-        <v>53.037304523682479</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+        <v>495.1323117529966</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
-        <v>32.910744385065506</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+        <v>270.65098135338718</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
-        <v>49.858730858364289</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+        <v>202.23302874402512</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
-        <v>122.25984699623346</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+        <v>17.228336541205209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
-        <v>17.424126353521867</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+        <v>293.14736412115303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
-        <v>4.998669169841305</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+        <v>917.41032383365769</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
-        <v>22.217274529854304</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+        <v>603.92169093038353</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
-        <v>15.190720452277159</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+        <v>738.5212072580531</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
-        <v>99.808928491923169</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+        <v>477.0478672900777</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
-        <v>46.681928579151801</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+        <v>282.11970954434173</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
-        <v>103.39372962361844</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+        <v>62.526205839080056</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
-        <v>55.150497949211733</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+        <v>127.08512986024229</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
-        <v>106.17963453359233</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+        <v>754.65342427585642</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
-        <v>65.01485812791104</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+        <v>484.63821550514228</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
-        <v>46.478628033583483</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+        <v>516.1840384933389</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
-        <v>126.45101676430077</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1105.8636427283679</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A80" s="3">
-        <v>68.296107377627919</v>
+        <v>300.2210100681645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>